<commit_message>
updated air quality data
</commit_message>
<xml_diff>
--- a/data/Air_Quality_Data.xlsx
+++ b/data/Air_Quality_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/86ea65660bb1531b/Documents/R/Applied-Spatial-Statistics-master/Final_Project/Air-Pollution-Correlates-4GA3.git/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iawan\OneDrive\Documents\AirPollution-4GA3\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="11_F25DC773A252ABDACC10484559DE414A5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCAFB576-2AEE-42B9-B642-3D350463681F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F21350D-7570-4B86-8686-D263D3CBED19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>COAVG</t>
+  </si>
+  <si>
+    <t>Oakwood Village Toronto</t>
+  </si>
+  <si>
+    <t>Moore Park</t>
   </si>
 </sst>
 </file>
@@ -161,10 +167,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -430,18 +432,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.44140625" customWidth="1"/>
+    <col min="1" max="1" width="45.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,7 +469,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -487,7 +489,7 @@
         <v>9.3333333333333339</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -507,7 +509,7 @@
         <v>8.6428571428571423</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -530,7 +532,7 @@
         <v>1.6428571428571428</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -553,7 +555,7 @@
         <v>1.6428571428571428</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -567,7 +569,7 @@
         <v>5.7967849999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -581,7 +583,7 @@
         <v>6.6035370000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -595,7 +597,7 @@
         <v>6.361415</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -609,7 +611,7 @@
         <v>6.687138</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -623,7 +625,7 @@
         <v>6.8196139999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -637,7 +639,7 @@
         <v>6.1986970000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -651,7 +653,7 @@
         <v>7.7694530000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -665,7 +667,7 @@
         <v>5.1035370000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -677,6 +679,48 @@
       </c>
       <c r="D14" s="1">
         <v>6.2479100000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>43.749099999999999</v>
+      </c>
+      <c r="C15">
+        <v>-79.440399999999997</v>
+      </c>
+      <c r="D15">
+        <v>1.0406060606060596</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>43.675699999999999</v>
+      </c>
+      <c r="C16">
+        <v>-79.418099999999995</v>
+      </c>
+      <c r="D16">
+        <v>6.5175595238095223</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17">
+        <v>43.751899999999999</v>
+      </c>
+      <c r="C17">
+        <v>-79.383399999999995</v>
+      </c>
+      <c r="D17">
+        <v>5.6800595238095228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Air Quality map to have 34 instead of 14 samples
</commit_message>
<xml_diff>
--- a/data/Air_Quality_Data.xlsx
+++ b/data/Air_Quality_Data.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iawan\OneDrive\Documents\AirPollution-4GA3\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\thaki\McMaster\ENVSOCTY 4GA3\Air-Pollution-Correlates-4GA3\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F21350D-7570-4B86-8686-D263D3CBED19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF67436F-3112-47BA-9787-F6600F6E6342}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -50,21 +50,30 @@
     <t>PM25Avg</t>
   </si>
   <si>
+    <t>O3AVG</t>
+  </si>
+  <si>
+    <t>NO2AVG</t>
+  </si>
+  <si>
     <t>SO2AVG</t>
   </si>
   <si>
-    <t>O3AVG</t>
-  </si>
-  <si>
-    <t>NO2AVG</t>
+    <t>COAVG</t>
   </si>
   <si>
     <t>Toronto East</t>
   </si>
   <si>
+    <t>NOTE: From 03/08/2024 20:00 - 03/21/2024 20:00</t>
+  </si>
+  <si>
     <t>Toronto North</t>
   </si>
   <si>
+    <t>Toronto</t>
+  </si>
+  <si>
     <t>Toronto West</t>
   </si>
   <si>
@@ -95,23 +104,71 @@
     <t>Harbour Terrace-1</t>
   </si>
   <si>
-    <t>Toronto</t>
-  </si>
-  <si>
-    <t>COAVG</t>
+    <t>South Ajax</t>
+  </si>
+  <si>
+    <t>Miyuu</t>
+  </si>
+  <si>
+    <t>Edgeleigh</t>
+  </si>
+  <si>
+    <t>MP19</t>
+  </si>
+  <si>
+    <t>MP21</t>
+  </si>
+  <si>
+    <t>MP5</t>
+  </si>
+  <si>
+    <t>MP26</t>
+  </si>
+  <si>
+    <t>MP13</t>
+  </si>
+  <si>
+    <t>Toronto Downtown (PurpleAir)</t>
+  </si>
+  <si>
+    <t>MP1</t>
+  </si>
+  <si>
+    <t>MP8</t>
+  </si>
+  <si>
+    <t>Moore Park</t>
   </si>
   <si>
     <t>Oakwood Village Toronto</t>
   </si>
   <si>
-    <t>Moore Park</t>
+    <t>Applewood Area</t>
+  </si>
+  <si>
+    <t>Toronto West-125 Resources RD</t>
+  </si>
+  <si>
+    <t>AQSU-401Roadside2</t>
+  </si>
+  <si>
+    <t>Toronto North - Downsview</t>
+  </si>
+  <si>
+    <t>Toronto Downtown (FEM)</t>
+  </si>
+  <si>
+    <t>AQSU-401Roadside1</t>
+  </si>
+  <si>
+    <t>AQSU-401Roadside3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +181,20 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -146,12 +217,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,18 +502,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.453125" customWidth="1"/>
+    <col min="1" max="1" width="45.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,21 +528,21 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
       <c r="H1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>43.747900000000001</v>
@@ -488,10 +559,13 @@
       <c r="F2">
         <v>9.3333333333333339</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>43.814100000000003</v>
@@ -509,9 +583,9 @@
         <v>8.6428571428571423</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>43.679400000000001</v>
@@ -532,9 +606,9 @@
         <v>1.6428571428571428</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>43.743400000000001</v>
@@ -555,51 +629,51 @@
         <v>1.6428571428571428</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B6">
-        <v>43.773699999999998</v>
+        <v>43.774679999999996</v>
       </c>
       <c r="C6">
-        <v>-79.507000000000005</v>
+        <v>-79.50703</v>
       </c>
       <c r="D6" s="1">
         <v>5.7967849999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B7">
-        <v>43.659199999999998</v>
+        <v>43.651820000000001</v>
       </c>
       <c r="C7">
-        <v>-79.406800000000004</v>
-      </c>
-      <c r="D7" s="2">
-        <v>6.6035370000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>-79.406739999999999</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6.5757190000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B8">
-        <v>43.653599999999997</v>
+        <v>43.646129999999999</v>
       </c>
       <c r="C8">
-        <v>-79.394000000000005</v>
+        <v>-79.393969999999996</v>
       </c>
       <c r="D8" s="1">
         <v>6.361415</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B9">
         <v>43.660899999999998</v>
@@ -611,51 +685,51 @@
         <v>6.687138</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B10">
-        <v>43.7029</v>
+        <v>43.687040000000003</v>
       </c>
       <c r="C10">
-        <v>-79.414199999999994</v>
+        <v>-79.414150000000006</v>
       </c>
       <c r="D10" s="1">
         <v>6.8196139999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B11">
-        <v>43.7181</v>
+        <v>43.685409999999997</v>
       </c>
       <c r="C11">
-        <v>-79.357299999999995</v>
+        <v>-79.357339999999994</v>
       </c>
       <c r="D11" s="1">
         <v>6.1986970000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B12">
-        <v>43.674900000000001</v>
+        <v>43.676020000000001</v>
       </c>
       <c r="C12">
-        <v>-79.354200000000006</v>
+        <v>-79.354339999999993</v>
       </c>
       <c r="D12" s="1">
         <v>7.7694530000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B13">
         <v>43.626800000000003</v>
@@ -667,9 +741,9 @@
         <v>5.1035370000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B14">
         <v>43.6372</v>
@@ -681,46 +755,288 @@
         <v>6.2479100000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15">
-        <v>43.749099999999999</v>
-      </c>
-      <c r="C15">
-        <v>-79.440399999999997</v>
-      </c>
-      <c r="D15">
-        <v>1.0406060606060596</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="2">
+        <v>43.830300000000001</v>
+      </c>
+      <c r="C15" s="2">
+        <v>-79.033159999999995</v>
+      </c>
+      <c r="D15" s="1">
+        <v>6.385942</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B16">
-        <v>43.675699999999999</v>
+        <v>43.827500000000001</v>
       </c>
       <c r="C16">
-        <v>-79.418099999999995</v>
-      </c>
-      <c r="D16">
-        <v>6.5175595238095223</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+        <v>-79.325699999999998</v>
+      </c>
+      <c r="D16" s="1">
+        <v>6.0431749999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B17">
-        <v>43.751899999999999</v>
+        <v>43.58</v>
       </c>
       <c r="C17">
-        <v>-79.383399999999995</v>
-      </c>
-      <c r="D17">
-        <v>5.6800595238095228</v>
+        <v>-79.561099999999996</v>
+      </c>
+      <c r="D17" s="1">
+        <v>4.9942489999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>43.662059999999997</v>
+      </c>
+      <c r="C18">
+        <v>-79.398420000000002</v>
+      </c>
+      <c r="D18" s="1">
+        <v>4.0210860000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>43.661900000000003</v>
+      </c>
+      <c r="C19">
+        <v>-79.398380000000003</v>
+      </c>
+      <c r="D19" s="1">
+        <v>3.5469650000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20">
+        <v>43.662430000000001</v>
+      </c>
+      <c r="C20">
+        <v>-79.39819</v>
+      </c>
+      <c r="D20" s="1">
+        <v>4.0389780000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21">
+        <v>43.662430000000001</v>
+      </c>
+      <c r="C21">
+        <v>-79.398480000000006</v>
+      </c>
+      <c r="D21" s="1">
+        <v>3.5444089999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22">
+        <v>43.661439999999999</v>
+      </c>
+      <c r="C22">
+        <v>-79.398020000000002</v>
+      </c>
+      <c r="D22" s="1">
+        <v>4.0383389999999997</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <v>43.662120000000002</v>
+      </c>
+      <c r="C23">
+        <v>-79.398330000000001</v>
+      </c>
+      <c r="D23" s="1">
+        <v>6.3293929999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24">
+        <v>43.662550000000003</v>
+      </c>
+      <c r="C24">
+        <v>-79.398079999999993</v>
+      </c>
+      <c r="D24" s="1">
+        <v>3.740256</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <v>43.670470000000002</v>
+      </c>
+      <c r="C25">
+        <v>-79.413510000000002</v>
+      </c>
+      <c r="D25" s="1">
+        <v>2.5878589999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26">
+        <v>43.691420000000001</v>
+      </c>
+      <c r="C26">
+        <v>-79.383309999999994</v>
+      </c>
+      <c r="D26" s="1">
+        <v>5.9492010000000004</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27">
+        <v>43.703000000000003</v>
+      </c>
+      <c r="C27">
+        <v>-79.440899999999999</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1.2364820000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28">
+        <v>43.658299999999997</v>
+      </c>
+      <c r="C28">
+        <v>-79.607600000000005</v>
+      </c>
+      <c r="D28" s="1">
+        <v>6.0096150000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29">
+        <v>43.710459999999998</v>
+      </c>
+      <c r="C29">
+        <v>-79.543549999999996</v>
+      </c>
+      <c r="D29" s="1">
+        <v>6.1022360000000004</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30">
+        <v>43.712150000000001</v>
+      </c>
+      <c r="C30">
+        <v>-79.543570000000003</v>
+      </c>
+      <c r="D30" s="1">
+        <v>7.9913740000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31">
+        <v>43.781559999999999</v>
+      </c>
+      <c r="C31">
+        <v>-79.467640000000003</v>
+      </c>
+      <c r="D31" s="1">
+        <v>5.6346150000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32">
+        <v>43.646509999999999</v>
+      </c>
+      <c r="C32">
+        <v>-79.389080000000007</v>
+      </c>
+      <c r="D32" s="1">
+        <v>7.2312700000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33">
+        <v>43.712200000000003</v>
+      </c>
+      <c r="C33">
+        <v>-79.543440000000004</v>
+      </c>
+      <c r="D33">
+        <v>7.3463258785942482</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <v>43.712200000000003</v>
+      </c>
+      <c r="C34">
+        <v>-79.543570000000003</v>
+      </c>
+      <c r="D34">
+        <v>5.7009584664536765</v>
       </c>
     </row>
   </sheetData>

</xml_diff>